<commit_message>
finished loan repayment fully - also finished bulc loan repayment and cron jobs for montlhy amount and loan interest calculator
</commit_message>
<xml_diff>
--- a/public/bulkfile/uploads/file/testl.xlsx
+++ b/public/bulkfile/uploads/file/testl.xlsx
@@ -17,6 +17,20 @@
     </ext>
   </extLst>
 </workbook>
+</file>
+
+<file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3" uniqueCount="3">
+  <si>
+    <t xml:space="preserve">loanno</t>
+  </si>
+  <si>
+    <t xml:space="preserve">memberno</t>
+  </si>
+  <si>
+    <t xml:space="preserve">amount</t>
+  </si>
+</sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
@@ -111,37 +125,224 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:C2"/>
+  <dimension ref="A1:C19"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C2" activeCellId="0" sqref="C2"/>
+      <selection pane="topLeft" activeCell="B1" activeCellId="0" sqref="B1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.5703125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.60546875" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="14.31"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A1" s="0" t="n">
-        <v>475838</v>
-      </c>
-      <c r="B1" s="0" t="n">
-        <v>111111</v>
-      </c>
-      <c r="C1" s="0" t="n">
-        <v>120000</v>
+      <c r="A1" s="0" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="0" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="0" t="s">
+        <v>2</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="0" t="n">
-        <v>813102</v>
+        <v>475838</v>
       </c>
       <c r="B2" s="0" t="n">
         <v>111111</v>
       </c>
       <c r="C2" s="0" t="n">
+        <v>120000</v>
+      </c>
+    </row>
+    <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A3" s="0" t="n">
+        <v>813102</v>
+      </c>
+      <c r="B3" s="0" t="n">
+        <v>111111</v>
+      </c>
+      <c r="C3" s="0" t="n">
         <v>16000</v>
+      </c>
+    </row>
+    <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A4" s="0" t="n">
+        <v>813103</v>
+      </c>
+      <c r="B4" s="0" t="n">
+        <v>111112</v>
+      </c>
+      <c r="C4" s="0" t="n">
+        <v>16001</v>
+      </c>
+    </row>
+    <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A5" s="0" t="n">
+        <v>813104</v>
+      </c>
+      <c r="B5" s="0" t="n">
+        <v>111113</v>
+      </c>
+      <c r="C5" s="0" t="n">
+        <v>16002</v>
+      </c>
+    </row>
+    <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A6" s="0" t="n">
+        <v>813105</v>
+      </c>
+      <c r="B6" s="0" t="n">
+        <v>111114</v>
+      </c>
+      <c r="C6" s="0" t="n">
+        <v>16003</v>
+      </c>
+    </row>
+    <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A7" s="0" t="n">
+        <v>813106</v>
+      </c>
+      <c r="B7" s="0" t="n">
+        <v>111115</v>
+      </c>
+      <c r="C7" s="0" t="n">
+        <v>16004</v>
+      </c>
+    </row>
+    <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A8" s="0" t="n">
+        <v>813107</v>
+      </c>
+      <c r="B8" s="0" t="n">
+        <v>111116</v>
+      </c>
+      <c r="C8" s="0" t="n">
+        <v>16005</v>
+      </c>
+    </row>
+    <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A9" s="0" t="n">
+        <v>813108</v>
+      </c>
+      <c r="B9" s="0" t="n">
+        <v>111117</v>
+      </c>
+      <c r="C9" s="0" t="n">
+        <v>16006</v>
+      </c>
+    </row>
+    <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A10" s="0" t="n">
+        <v>813109</v>
+      </c>
+      <c r="B10" s="0" t="n">
+        <v>111118</v>
+      </c>
+      <c r="C10" s="0" t="n">
+        <v>16007</v>
+      </c>
+    </row>
+    <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A11" s="0" t="n">
+        <v>813110</v>
+      </c>
+      <c r="B11" s="0" t="n">
+        <v>111119</v>
+      </c>
+      <c r="C11" s="0" t="n">
+        <v>16008</v>
+      </c>
+    </row>
+    <row r="12" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A12" s="0" t="n">
+        <v>813111</v>
+      </c>
+      <c r="B12" s="0" t="n">
+        <v>111120</v>
+      </c>
+      <c r="C12" s="0" t="n">
+        <v>16009</v>
+      </c>
+    </row>
+    <row r="13" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A13" s="0" t="n">
+        <v>813112</v>
+      </c>
+      <c r="B13" s="0" t="n">
+        <v>111121</v>
+      </c>
+      <c r="C13" s="0" t="n">
+        <v>16010</v>
+      </c>
+    </row>
+    <row r="14" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A14" s="0" t="n">
+        <v>813113</v>
+      </c>
+      <c r="B14" s="0" t="n">
+        <v>111122</v>
+      </c>
+      <c r="C14" s="0" t="n">
+        <v>16011</v>
+      </c>
+    </row>
+    <row r="15" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A15" s="0" t="n">
+        <v>813114</v>
+      </c>
+      <c r="B15" s="0" t="n">
+        <v>111123</v>
+      </c>
+      <c r="C15" s="0" t="n">
+        <v>16012</v>
+      </c>
+    </row>
+    <row r="16" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A16" s="0" t="n">
+        <v>813115</v>
+      </c>
+      <c r="B16" s="0" t="n">
+        <v>111124</v>
+      </c>
+      <c r="C16" s="0" t="n">
+        <v>16013</v>
+      </c>
+    </row>
+    <row r="17" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A17" s="0" t="n">
+        <v>813116</v>
+      </c>
+      <c r="B17" s="0" t="n">
+        <v>111125</v>
+      </c>
+      <c r="C17" s="0" t="n">
+        <v>16014</v>
+      </c>
+    </row>
+    <row r="18" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A18" s="0" t="n">
+        <v>813117</v>
+      </c>
+      <c r="B18" s="0" t="n">
+        <v>111126</v>
+      </c>
+      <c r="C18" s="0" t="n">
+        <v>16015</v>
+      </c>
+    </row>
+    <row r="19" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A19" s="0" t="n">
+        <v>813118</v>
+      </c>
+      <c r="B19" s="0" t="n">
+        <v>111127</v>
+      </c>
+      <c r="C19" s="0" t="n">
+        <v>16016</v>
       </c>
     </row>
   </sheetData>

</xml_diff>